<commit_message>
réglage gros bug de variable global et aussi JM
</commit_message>
<xml_diff>
--- a/output_results/beta/beta_results.xlsx
+++ b/output_results/beta/beta_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="15">
   <si>
     <t>nCandidates:</t>
   </si>
@@ -53,6 +53,12 @@
   </si>
   <si>
     <t>Montebourg</t>
+  </si>
+  <si>
+    <t>Macron</t>
+  </si>
+  <si>
+    <t>Philipot</t>
   </si>
 </sst>
 </file>
@@ -410,41 +416,43 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AW12"/>
+  <dimension ref="A1:AQ12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:49">
+    <row r="1" spans="1:43">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1">
+        <v>4</v>
+      </c>
       <c r="I1" s="1"/>
-      <c r="J1" s="1">
-        <v>5</v>
-      </c>
+      <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="N1" s="1">
+        <v>6</v>
+      </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1">
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1">
         <v>8</v>
       </c>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
       <c r="U1" s="1"/>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
@@ -458,86 +466,80 @@
       <c r="AC1" s="1"/>
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
-      <c r="AF1" s="1"/>
+      <c r="AF1" s="1">
+        <v>12</v>
+      </c>
       <c r="AG1" s="1"/>
-      <c r="AH1" s="1">
-        <v>12</v>
-      </c>
+      <c r="AH1" s="1"/>
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
-      <c r="AL1" s="1"/>
+      <c r="AL1" s="1">
+        <v>14</v>
+      </c>
       <c r="AM1" s="1"/>
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
-      <c r="AP1" s="1">
-        <v>14</v>
-      </c>
+      <c r="AP1" s="1"/>
       <c r="AQ1" s="1"/>
-      <c r="AR1" s="1"/>
-      <c r="AS1" s="1"/>
-      <c r="AT1" s="1"/>
-      <c r="AU1" s="1"/>
-      <c r="AV1" s="1"/>
-      <c r="AW1" s="1"/>
     </row>
-    <row r="2" spans="1:49">
+    <row r="2" spans="1:43">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1">
+        <v>100</v>
+      </c>
+      <c r="E2" s="1">
+        <v>500</v>
+      </c>
+      <c r="F2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="G2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="H2" s="1">
         <v>10</v>
       </c>
-      <c r="E2" s="1">
+      <c r="I2" s="1">
         <v>50</v>
       </c>
-      <c r="F2" s="1">
+      <c r="J2" s="1">
         <v>100</v>
       </c>
-      <c r="G2" s="1">
+      <c r="K2" s="1">
         <v>500</v>
       </c>
-      <c r="H2" s="1">
+      <c r="L2" s="1">
         <v>1000</v>
       </c>
-      <c r="I2" s="1">
+      <c r="M2" s="1">
         <v>10000</v>
       </c>
-      <c r="J2" s="1">
-        <v>3</v>
-      </c>
-      <c r="K2" s="1">
-        <v>5</v>
-      </c>
-      <c r="L2" s="1">
+      <c r="N2" s="1">
         <v>10</v>
       </c>
-      <c r="M2" s="1">
+      <c r="O2" s="1">
         <v>50</v>
       </c>
-      <c r="N2" s="1">
+      <c r="P2" s="1">
         <v>100</v>
       </c>
-      <c r="O2" s="1">
+      <c r="Q2" s="1">
         <v>500</v>
       </c>
-      <c r="P2" s="1">
+      <c r="R2" s="1">
         <v>1000</v>
       </c>
-      <c r="Q2" s="1">
+      <c r="S2" s="1">
         <v>10000</v>
-      </c>
-      <c r="R2" s="1">
-        <v>3</v>
-      </c>
-      <c r="S2" s="1">
-        <v>5</v>
       </c>
       <c r="T2" s="1">
         <v>10</v>
@@ -558,90 +560,69 @@
         <v>10000</v>
       </c>
       <c r="Z2" s="1">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="AA2" s="1">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="AB2" s="1">
+        <v>100</v>
+      </c>
+      <c r="AC2" s="1">
+        <v>500</v>
+      </c>
+      <c r="AD2" s="1">
+        <v>1000</v>
+      </c>
+      <c r="AE2" s="1">
+        <v>10000</v>
+      </c>
+      <c r="AF2" s="1">
         <v>10</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AG2" s="1">
         <v>50</v>
       </c>
-      <c r="AD2" s="1">
+      <c r="AH2" s="1">
         <v>100</v>
       </c>
-      <c r="AE2" s="1">
+      <c r="AI2" s="1">
         <v>500</v>
       </c>
-      <c r="AF2" s="1">
+      <c r="AJ2" s="1">
         <v>1000</v>
       </c>
-      <c r="AG2" s="1">
+      <c r="AK2" s="1">
         <v>10000</v>
       </c>
-      <c r="AH2" s="1">
-        <v>3</v>
-      </c>
-      <c r="AI2" s="1">
-        <v>5</v>
-      </c>
-      <c r="AJ2" s="1">
+      <c r="AL2" s="1">
         <v>10</v>
       </c>
-      <c r="AK2" s="1">
+      <c r="AM2" s="1">
         <v>50</v>
       </c>
-      <c r="AL2" s="1">
+      <c r="AN2" s="1">
         <v>100</v>
       </c>
-      <c r="AM2" s="1">
+      <c r="AO2" s="1">
         <v>500</v>
       </c>
-      <c r="AN2" s="1">
+      <c r="AP2" s="1">
         <v>1000</v>
       </c>
-      <c r="AO2" s="1">
+      <c r="AQ2" s="1">
         <v>10000</v>
       </c>
-      <c r="AP2" s="1">
-        <v>3</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>5</v>
-      </c>
-      <c r="AR2" s="1">
-        <v>10</v>
-      </c>
-      <c r="AS2" s="1">
-        <v>50</v>
-      </c>
-      <c r="AT2" s="1">
-        <v>100</v>
-      </c>
-      <c r="AU2" s="1">
-        <v>500</v>
-      </c>
-      <c r="AV2" s="1">
-        <v>1000</v>
-      </c>
-      <c r="AW2" s="1">
-        <v>10000</v>
-      </c>
     </row>
-    <row r="3" spans="1:49">
+    <row r="3" spans="1:43">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:49">
+    <row r="4" spans="1:43">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
@@ -658,7 +639,7 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I4" t="s">
         <v>12</v>
@@ -676,7 +657,7 @@
         <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O4" t="s">
         <v>12</v>
@@ -694,7 +675,7 @@
         <v>12</v>
       </c>
       <c r="T4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U4" t="s">
         <v>12</v>
@@ -712,7 +693,7 @@
         <v>12</v>
       </c>
       <c r="Z4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AA4" t="s">
         <v>12</v>
@@ -730,7 +711,7 @@
         <v>12</v>
       </c>
       <c r="AF4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AG4" t="s">
         <v>12</v>
@@ -748,7 +729,7 @@
         <v>12</v>
       </c>
       <c r="AL4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AM4" t="s">
         <v>12</v>
@@ -765,26 +746,8 @@
       <c r="AQ4" t="s">
         <v>12</v>
       </c>
-      <c r="AR4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>12</v>
-      </c>
-      <c r="AW4" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="5" spans="1:49">
+    <row r="5" spans="1:43">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
@@ -914,26 +877,8 @@
       <c r="AQ5" t="s">
         <v>12</v>
       </c>
-      <c r="AR5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>12</v>
-      </c>
-      <c r="AW5" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="6" spans="1:49">
+    <row r="6" spans="1:43">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1063,26 +1008,8 @@
       <c r="AQ6" t="s">
         <v>12</v>
       </c>
-      <c r="AR6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV6" t="s">
-        <v>12</v>
-      </c>
-      <c r="AW6" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="7" spans="1:49">
+    <row r="7" spans="1:43">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1123,7 +1050,7 @@
         <v>12</v>
       </c>
       <c r="N7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O7" t="s">
         <v>12</v>
@@ -1141,7 +1068,7 @@
         <v>12</v>
       </c>
       <c r="T7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U7" t="s">
         <v>12</v>
@@ -1177,7 +1104,7 @@
         <v>12</v>
       </c>
       <c r="AF7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AG7" t="s">
         <v>12</v>
@@ -1195,7 +1122,7 @@
         <v>12</v>
       </c>
       <c r="AL7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AM7" t="s">
         <v>12</v>
@@ -1212,26 +1139,8 @@
       <c r="AQ7" t="s">
         <v>12</v>
       </c>
-      <c r="AR7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV7" t="s">
-        <v>12</v>
-      </c>
-      <c r="AW7" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="8" spans="1:49">
+    <row r="8" spans="1:43">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1272,7 +1181,7 @@
         <v>12</v>
       </c>
       <c r="N8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O8" t="s">
         <v>12</v>
@@ -1290,7 +1199,7 @@
         <v>12</v>
       </c>
       <c r="T8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U8" t="s">
         <v>12</v>
@@ -1326,7 +1235,7 @@
         <v>12</v>
       </c>
       <c r="AF8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AG8" t="s">
         <v>12</v>
@@ -1344,7 +1253,7 @@
         <v>12</v>
       </c>
       <c r="AL8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AM8" t="s">
         <v>12</v>
@@ -1361,26 +1270,8 @@
       <c r="AQ8" t="s">
         <v>12</v>
       </c>
-      <c r="AR8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV8" t="s">
-        <v>12</v>
-      </c>
-      <c r="AW8" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="9" spans="1:49">
+    <row r="9" spans="1:43">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1457,7 +1348,7 @@
         <v>12</v>
       </c>
       <c r="Z9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AA9" t="s">
         <v>12</v>
@@ -1475,7 +1366,7 @@
         <v>12</v>
       </c>
       <c r="AF9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AG9" t="s">
         <v>12</v>
@@ -1493,7 +1384,7 @@
         <v>12</v>
       </c>
       <c r="AL9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="AM9" t="s">
         <v>12</v>
@@ -1510,31 +1401,13 @@
       <c r="AQ9" t="s">
         <v>12</v>
       </c>
-      <c r="AR9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV9" t="s">
-        <v>12</v>
-      </c>
-      <c r="AW9" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="10" spans="1:49">
+    <row r="10" spans="1:43">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -1552,7 +1425,7 @@
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I10" t="s">
         <v>12</v>
@@ -1570,7 +1443,7 @@
         <v>12</v>
       </c>
       <c r="N10" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O10" t="s">
         <v>12</v>
@@ -1588,7 +1461,7 @@
         <v>12</v>
       </c>
       <c r="T10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U10" t="s">
         <v>12</v>
@@ -1606,7 +1479,7 @@
         <v>12</v>
       </c>
       <c r="Z10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AA10" t="s">
         <v>12</v>
@@ -1624,7 +1497,7 @@
         <v>12</v>
       </c>
       <c r="AF10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AG10" t="s">
         <v>12</v>
@@ -1642,7 +1515,7 @@
         <v>12</v>
       </c>
       <c r="AL10" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AM10" t="s">
         <v>12</v>
@@ -1659,31 +1532,13 @@
       <c r="AQ10" t="s">
         <v>12</v>
       </c>
-      <c r="AR10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV10" t="s">
-        <v>12</v>
-      </c>
-      <c r="AW10" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="11" spans="1:49">
+    <row r="11" spans="1:43">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1701,7 +1556,7 @@
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="I11" t="s">
         <v>12</v>
@@ -1719,7 +1574,7 @@
         <v>12</v>
       </c>
       <c r="N11" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O11" t="s">
         <v>12</v>
@@ -1737,7 +1592,7 @@
         <v>12</v>
       </c>
       <c r="T11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U11" t="s">
         <v>12</v>
@@ -1755,7 +1610,7 @@
         <v>12</v>
       </c>
       <c r="Z11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AA11" t="s">
         <v>12</v>
@@ -1773,7 +1628,7 @@
         <v>12</v>
       </c>
       <c r="AF11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AG11" t="s">
         <v>12</v>
@@ -1791,7 +1646,7 @@
         <v>12</v>
       </c>
       <c r="AL11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AM11" t="s">
         <v>12</v>
@@ -1808,26 +1663,8 @@
       <c r="AQ11" t="s">
         <v>12</v>
       </c>
-      <c r="AR11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV11" t="s">
-        <v>12</v>
-      </c>
-      <c r="AW11" t="s">
-        <v>12</v>
-      </c>
     </row>
-    <row r="12" spans="1:49">
+    <row r="12" spans="1:43">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1868,7 +1705,7 @@
         <v>12</v>
       </c>
       <c r="N12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O12" t="s">
         <v>12</v>
@@ -1886,7 +1723,7 @@
         <v>12</v>
       </c>
       <c r="T12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="U12" t="s">
         <v>12</v>
@@ -1922,7 +1759,7 @@
         <v>12</v>
       </c>
       <c r="AF12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AG12" t="s">
         <v>12</v>
@@ -1940,7 +1777,7 @@
         <v>12</v>
       </c>
       <c r="AL12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AM12" t="s">
         <v>12</v>
@@ -1955,35 +1792,18 @@
         <v>12</v>
       </c>
       <c r="AQ12" t="s">
-        <v>12</v>
-      </c>
-      <c r="AR12" t="s">
-        <v>12</v>
-      </c>
-      <c r="AS12" t="s">
-        <v>12</v>
-      </c>
-      <c r="AT12" t="s">
-        <v>12</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>12</v>
-      </c>
-      <c r="AV12" t="s">
-        <v>12</v>
-      </c>
-      <c r="AW12" t="s">
         <v>12</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B1:I1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="R1:Y1"/>
-    <mergeCell ref="Z1:AG1"/>
-    <mergeCell ref="AH1:AO1"/>
-    <mergeCell ref="AP1:AW1"/>
+  <mergeCells count="7">
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="N1:S1"/>
+    <mergeCell ref="T1:Y1"/>
+    <mergeCell ref="Z1:AE1"/>
+    <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="AL1:AQ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
last commit & move rapport
</commit_message>
<xml_diff>
--- a/output_results/beta/beta_results.xlsx
+++ b/output_results/beta/beta_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="14">
   <si>
     <t>nCandidates:</t>
   </si>
@@ -50,18 +50,6 @@
   </si>
   <si>
     <t>Vote de Copeland</t>
-  </si>
-  <si>
-    <t>Zemmour</t>
-  </si>
-  <si>
-    <t>Hidalgo</t>
-  </si>
-  <si>
-    <t>Pécresse</t>
-  </si>
-  <si>
-    <t>Jadot</t>
   </si>
   <si>
     <t>Montebourg</t>
@@ -632,11 +620,8 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
       <c r="C4" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -651,112 +636,112 @@
         <v>12</v>
       </c>
       <c r="H4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I4" t="s">
         <v>13</v>
       </c>
       <c r="J4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="P4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Q4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="R4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="W4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Y4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AA4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AB4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AC4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AD4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AE4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AF4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AG4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AH4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AI4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AJ4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AK4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AL4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AM4" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AN4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AO4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AP4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AQ4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:43">
@@ -767,7 +752,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -782,112 +767,112 @@
         <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I5" t="s">
         <v>13</v>
       </c>
       <c r="J5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="P5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Q5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="R5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="S5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="T5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="V5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="W5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="X5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Y5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Z5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AA5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AB5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AC5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AD5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AE5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AF5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="AG5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AH5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AI5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AJ5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AK5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AL5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AM5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AN5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AO5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AP5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AQ5" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -898,7 +883,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -913,112 +898,112 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I6" t="s">
         <v>13</v>
       </c>
       <c r="J6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="P6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="R6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="S6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="T6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="W6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="X6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="Y6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Z6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AA6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AB6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AC6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AD6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AE6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AF6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="AG6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AH6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AI6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AJ6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AK6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AL6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="AM6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AN6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AO6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AP6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AQ6" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -1029,7 +1014,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1044,112 +1029,112 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="P7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="R7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="W7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Y7" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AA7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AB7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AC7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AD7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AE7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AF7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AG7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AH7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AI7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AJ7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AK7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AL7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AM7" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AN7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AO7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AP7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AQ7" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -1160,7 +1145,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1175,112 +1160,112 @@
         <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="P8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="R8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T8" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="U8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="V8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="W8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Y8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AA8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AB8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AC8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AD8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AE8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AF8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AG8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AH8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AI8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AJ8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AK8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AL8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AM8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AN8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AO8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AP8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AQ8" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -1291,7 +1276,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -1306,112 +1291,112 @@
         <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I9" t="s">
         <v>13</v>
       </c>
       <c r="J9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="P9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Q9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="R9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="U9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="V9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="W9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Y9" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AA9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AB9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AC9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AD9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AE9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AF9" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="AG9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AH9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AI9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AJ9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AK9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AL9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AM9" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="AN9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AO9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AP9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AQ9" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:43">
@@ -1437,112 +1422,112 @@
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M10" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="O10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="P10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="R10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="U10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="V10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="W10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Y10" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AA10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AB10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AC10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AD10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AE10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AF10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AG10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AH10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AI10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AJ10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AK10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AL10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AM10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AN10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AO10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AP10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AQ10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:43">
@@ -1568,112 +1553,112 @@
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="O11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="P11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="R11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="U11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="V11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="W11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Y11" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AA11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AB11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AC11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AD11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AE11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AF11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="AG11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AH11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AI11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AJ11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AK11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AL11" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="AM11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AN11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AO11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AP11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AQ11" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:43">
@@ -1684,7 +1669,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -1699,112 +1684,112 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="I12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="M12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="N12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="O12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="P12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Q12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="R12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="S12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="T12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="U12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="V12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="W12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="X12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Y12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AA12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AB12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AC12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AD12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AE12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AF12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AG12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AH12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AI12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AJ12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AK12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AL12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AM12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AN12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AO12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AP12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="AQ12" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
séparation simulation / méthodes, en 2 fichiers
</commit_message>
<xml_diff>
--- a/output_results/beta/beta_results.xlsx
+++ b/output_results/beta/beta_results.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="389" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="18">
   <si>
     <t>nCandidates:</t>
   </si>
@@ -52,10 +52,22 @@
     <t>Vote de Copeland</t>
   </si>
   <si>
-    <t>Montebourg</t>
+    <t>Jadot</t>
+  </si>
+  <si>
+    <t>Zemmour</t>
+  </si>
+  <si>
+    <t>Pécresse</t>
+  </si>
+  <si>
+    <t>Macron</t>
   </si>
   <si>
     <t>Philipot</t>
+  </si>
+  <si>
+    <t>Montebourg</t>
   </si>
 </sst>
 </file>
@@ -620,8 +632,11 @@
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
       <c r="C4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D4" t="s">
         <v>12</v>
@@ -639,109 +654,109 @@
         <v>12</v>
       </c>
       <c r="I4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N4" t="s">
         <v>12</v>
       </c>
       <c r="O4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="T4" t="s">
         <v>12</v>
       </c>
       <c r="U4" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="V4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="W4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Y4" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AA4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AB4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AC4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AD4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AE4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AF4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AG4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AH4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AI4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AJ4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AK4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AL4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AM4" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AN4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AO4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AP4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AQ4" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:43">
@@ -752,7 +767,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
@@ -767,13 +782,13 @@
         <v>12</v>
       </c>
       <c r="H5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K5" t="s">
         <v>12</v>
@@ -785,10 +800,10 @@
         <v>12</v>
       </c>
       <c r="N5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="O5" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P5" t="s">
         <v>12</v>
@@ -803,76 +818,76 @@
         <v>12</v>
       </c>
       <c r="T5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="V5" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="W5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Y5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AA5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AB5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AC5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AD5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AE5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AF5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AG5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AH5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AI5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AJ5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AK5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AL5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AM5" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AN5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AO5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AP5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AQ5" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:43">
@@ -883,7 +898,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
         <v>12</v>
@@ -898,112 +913,112 @@
         <v>12</v>
       </c>
       <c r="H6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M6" t="s">
         <v>12</v>
       </c>
       <c r="N6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="O6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Q6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S6" t="s">
         <v>12</v>
       </c>
       <c r="T6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="V6" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="W6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Y6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AA6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AB6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AC6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AD6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AE6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AF6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AG6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AH6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AI6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AJ6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AK6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AL6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AM6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AN6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AO6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AP6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AQ6" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:43">
@@ -1011,10 +1026,10 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D7" t="s">
         <v>12</v>
@@ -1029,112 +1044,112 @@
         <v>12</v>
       </c>
       <c r="H7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="O7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="P7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="T7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="U7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="V7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="W7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Y7" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AA7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AB7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AC7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AD7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AE7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AF7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AG7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AH7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AI7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AJ7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AK7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AL7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AM7" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AN7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AO7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AP7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AQ7" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:43">
@@ -1145,7 +1160,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
         <v>12</v>
@@ -1160,112 +1175,112 @@
         <v>12</v>
       </c>
       <c r="H8" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="T8" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="U8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="V8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="W8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Y8" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AA8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AB8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AC8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AD8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AE8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AF8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AG8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AH8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AI8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AJ8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AK8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AL8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AM8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AN8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AO8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AP8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AQ8" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:43">
@@ -1276,7 +1291,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9" t="s">
         <v>12</v>
@@ -1291,112 +1306,112 @@
         <v>12</v>
       </c>
       <c r="H9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="J9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="O9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="P9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="Q9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="T9" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U9" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="V9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="W9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Y9" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AA9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AB9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AC9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AD9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AE9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AF9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AG9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AH9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AI9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AJ9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AK9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AL9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AM9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="AN9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AO9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AP9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AQ9" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:43">
@@ -1422,112 +1437,112 @@
         <v>12</v>
       </c>
       <c r="H10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M10" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="O10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="T10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="U10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="V10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="W10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Y10" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AA10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AB10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AC10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AD10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AE10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AF10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AG10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AH10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AI10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AJ10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AK10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AL10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AM10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AN10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AO10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AP10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AQ10" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:43">
@@ -1553,112 +1568,112 @@
         <v>12</v>
       </c>
       <c r="H11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M11" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="O11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="T11" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="U11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="V11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="W11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Y11" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AA11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AB11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AC11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AD11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AE11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AF11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AG11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AH11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AI11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AJ11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AK11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AL11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AM11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AN11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AO11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AP11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AQ11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:43">
@@ -1669,7 +1684,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12" t="s">
         <v>12</v>
@@ -1684,112 +1699,112 @@
         <v>12</v>
       </c>
       <c r="H12" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="I12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="J12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="K12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="L12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="M12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="N12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="O12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="P12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Q12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="R12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="S12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="T12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="U12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="V12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="W12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="X12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Y12" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="Z12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AA12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AB12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AC12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AD12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AE12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AF12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AG12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AH12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AI12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AJ12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AK12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AL12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AM12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AN12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AO12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AP12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="AQ12" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>